<commit_message>
Add mapping for zib Pregnancy
</commit_message>
<xml_diff>
--- a/Mappings/Pregnancy - STU3.xlsx
+++ b/Mappings/Pregnancy - STU3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edelman\Nictiz-STU3-Zib2017\Mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2001BC49-6469-44AB-8041-78886D2D6FC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028C48AA-B353-4BBB-8723-144F58D61AC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="163">
   <si>
     <t>Subject</t>
   </si>
@@ -459,26 +459,61 @@
     <t>pregnancy</t>
   </si>
   <si>
-    <t>HCIM Alert
-Pregnancy status, outcome and expected delivery date profiles from the  International Patient Summary (IPS)</t>
-  </si>
-  <si>
-    <t>Pregnancy is in this model a flag to pay extra attention during care. However, this is just a flag that points to another resoure for details
-Status and EDD overlap with this HCIM. Perhaps it's useful to leverage this? However, IPS is in development and these fields are quite simple, primitve fields</t>
-  </si>
-  <si>
     <t>Pregnancy is mentioned as an example of a Condition</t>
   </si>
   <si>
-    <t>https://chat.fhir.org/#narrow/stream/179166-implementers/topic/Mother.2FChild.20record
-https://chat.fhir.org/#narrow/stream/implementers/topic/FHIR.20Resource.20for.20Pregnancy.20Episode</t>
-  </si>
-  <si>
-    <t>The question is whether this HCIM actually maps to a Condition. Although the fields map quite well, the intent is to use it as a point-in-time status for care purposes. An Observation might be better suited for this purpose. OTOH, Observation might preclude other use cases(?)</t>
-  </si>
-  <si>
-    <t>This discussion focuses on the question how to relate a child record to a mother record and is not really relevant to us
-This discussion raises the isue that EDD and LMP might actually be better represented as a more complex Observation rather than with primitive DateTime fields</t>
+    <t>HCIM Alert</t>
+  </si>
+  <si>
+    <t>Pregnancy status, outcome and expected delivery date profiles from the  International Patient Summary (IPS)</t>
+  </si>
+  <si>
+    <t>Pregnancy is in this model a flag to pay extra attention during care. However, this is just a flag that points to another resoure for details</t>
+  </si>
+  <si>
+    <t>Status and EDD overlap with this HCIM. Perhaps it's useful to leverage this? However, IPS is in development and these fields are quite simple, primitve fields</t>
+  </si>
+  <si>
+    <t>https://chat.fhir.org/#narrow/stream/implementers/topic/FHIR.20Resource.20for.20Pregnancy.20Episode</t>
+  </si>
+  <si>
+    <t>https://chat.fhir.org/#narrow/stream/179166-implementers/topic/Mother.2FChild.20record</t>
+  </si>
+  <si>
+    <t>This discussion focuses on the question how to relate a child record to a mother record and is not really relevant to us</t>
+  </si>
+  <si>
+    <t>This discussion raises the isue that EDD and LMP might actually be better represented as a more complex Observation rather than with primitive DateTime fields</t>
+  </si>
+  <si>
+    <t>The fields of this HCIM fit quite well to Condition. However, the question is if Observation might be better suited. See the notes on the Data tab for more information</t>
+  </si>
+  <si>
+    <t>.valueBoolean</t>
+  </si>
+  <si>
+    <t>.comment</t>
+  </si>
+  <si>
+    <t>.component / slice TermDate (DateTime)</t>
+  </si>
+  <si>
+    <t>.component / slice DateLastMenstruation (DateTime)</t>
+  </si>
+  <si>
+    <t>.component / slice PregnancyDuration (quantity)</t>
+  </si>
+  <si>
+    <t>.component / slice Gravidity (quantity)</t>
+  </si>
+  <si>
+    <t>.component / slice Parity (quantity)</t>
+  </si>
+  <si>
+    <t>nl-core-observation (DefinitionCode on .code)</t>
+  </si>
+  <si>
+    <t>The question is whether this HCIM maps to a Condition or an Observation. The fields map quite well on Condition and pregnancy is even mentioned as an example of a Condition. However, the intent of this HCIM is to use it as measurement of the current status, so we'll use an Observation. These observations might be grouped together in an HCIM Problem to track the overaching situation.</t>
   </si>
 </sst>
 </file>
@@ -522,7 +557,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -537,6 +572,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE3E3E3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -604,7 +645,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -648,15 +689,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -934,15 +984,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1001,15 +1051,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1068,15 +1118,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1135,15 +1185,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1202,15 +1252,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1269,15 +1319,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1336,15 +1386,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1403,15 +1453,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1470,15 +1520,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1537,15 +1587,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1604,15 +1654,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>190500</xdr:rowOff>
+          <xdr:rowOff>200025</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1671,15 +1721,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>190500</xdr:rowOff>
+          <xdr:rowOff>200025</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1738,15 +1788,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>363855</xdr:rowOff>
+          <xdr:rowOff>371475</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1805,15 +1855,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>363855</xdr:rowOff>
+          <xdr:rowOff>371475</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1872,15 +1922,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>363855</xdr:rowOff>
+          <xdr:rowOff>371475</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1939,15 +1989,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>363855</xdr:rowOff>
+          <xdr:rowOff>371475</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2006,15 +2056,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>363855</xdr:rowOff>
+          <xdr:rowOff>371475</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2073,15 +2123,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>363855</xdr:rowOff>
+          <xdr:rowOff>371475</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2140,15 +2190,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>358140</xdr:rowOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2207,15 +2257,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>358140</xdr:rowOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2274,15 +2324,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>53340</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>129540</xdr:rowOff>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>358140</xdr:rowOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2341,15 +2391,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>53340</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>129540</xdr:rowOff>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>358140</xdr:rowOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2408,15 +2458,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>358140</xdr:rowOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2475,15 +2525,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>358140</xdr:rowOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2542,15 +2592,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
-          <xdr:row>9</xdr:row>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>10</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>53340</xdr:rowOff>
+          <xdr:rowOff>219075</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2609,15 +2659,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
-          <xdr:row>9</xdr:row>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>10</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>53340</xdr:rowOff>
+          <xdr:rowOff>219075</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2676,15 +2726,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>53340</xdr:colOff>
-          <xdr:row>9</xdr:row>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>10</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>59055</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2743,15 +2793,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>53340</xdr:colOff>
-          <xdr:row>9</xdr:row>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>10</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>59055</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2810,15 +2860,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
-          <xdr:row>9</xdr:row>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>10</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>53340</xdr:rowOff>
+          <xdr:rowOff>219075</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2877,15 +2927,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
-          <xdr:row>9</xdr:row>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>10</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>53340</xdr:rowOff>
+          <xdr:rowOff>219075</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2944,15 +2994,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3011,15 +3061,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3077,7 +3127,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3377,13 +3427,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3391,7 +3441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -3399,7 +3449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -3407,7 +3457,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -3415,7 +3465,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -3423,7 +3473,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -3431,7 +3481,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -3439,7 +3489,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
@@ -3447,7 +3497,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
@@ -3455,7 +3505,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
@@ -3463,7 +3513,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" ht="51" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>55</v>
       </c>
@@ -3471,7 +3521,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>57</v>
       </c>
@@ -3479,7 +3529,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>59</v>
       </c>
@@ -3505,19 +3555,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="17" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="17"/>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C2" s="20"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
@@ -3525,7 +3575,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
@@ -3533,7 +3583,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
@@ -3541,7 +3591,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
@@ -3549,7 +3599,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -3557,7 +3607,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
@@ -3565,13 +3615,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
@@ -3579,13 +3629,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
@@ -3593,13 +3643,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>37</v>
       </c>
@@ -3607,7 +3657,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>39</v>
       </c>
@@ -3615,7 +3665,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>41</v>
       </c>
@@ -3623,7 +3673,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>42</v>
       </c>
@@ -3631,7 +3681,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>43</v>
       </c>
@@ -3639,7 +3689,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
@@ -3647,7 +3697,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
@@ -3655,7 +3705,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
@@ -3663,7 +3713,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>49</v>
       </c>
@@ -3671,7 +3721,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>50</v>
       </c>
@@ -3679,7 +3729,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>52</v>
       </c>
@@ -3687,7 +3737,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>53</v>
       </c>
@@ -3712,9 +3762,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
     </row>
   </sheetData>
@@ -3725,22 +3775,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515DB529-7A3E-4DDA-9800-41676C7906CF}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.21875" customWidth="1"/>
+    <col min="1" max="1" width="40.28515625" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" customWidth="1"/>
-    <col min="4" max="4" width="85.6640625" customWidth="1"/>
-    <col min="5" max="5" width="127.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="85.7109375" customWidth="1"/>
+    <col min="5" max="5" width="95.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>127</v>
       </c>
@@ -3757,7 +3807,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>132</v>
       </c>
@@ -3765,29 +3815,31 @@
         <v>143</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>133</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E3" s="18"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>141</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4" s="18"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>134</v>
       </c>
@@ -3797,8 +3849,9 @@
       <c r="D5" s="16" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5" s="18"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>135</v>
       </c>
@@ -3808,42 +3861,62 @@
       <c r="D6" s="16" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6" s="18"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="18"/>
+    </row>
+    <row r="8" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>137</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="E8" s="18" t="s">
+      <c r="D8" s="17" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
+      <c r="E8" s="17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C10" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="E9" s="18" t="s">
+      <c r="D10" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
+      <c r="E11" s="18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3862,15 +3935,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>0</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:row>1</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3884,15 +3957,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3906,15 +3979,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
-                    <xdr:row>3</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3928,15 +4001,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>0</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:row>1</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3950,15 +4023,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3972,15 +4045,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3994,15 +4067,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4016,15 +4089,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4038,15 +4111,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4060,15 +4133,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4082,15 +4155,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>198120</xdr:rowOff>
+                    <xdr:rowOff>200025</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4104,15 +4177,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>198120</xdr:rowOff>
+                    <xdr:rowOff>200025</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4126,15 +4199,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>373380</xdr:rowOff>
+                    <xdr:rowOff>371475</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4148,15 +4221,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>373380</xdr:rowOff>
+                    <xdr:rowOff>371475</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4170,15 +4243,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>373380</xdr:rowOff>
+                    <xdr:rowOff>371475</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4192,15 +4265,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>373380</xdr:rowOff>
+                    <xdr:rowOff>371475</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4214,15 +4287,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>373380</xdr:rowOff>
+                    <xdr:rowOff>371475</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4236,15 +4309,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>373380</xdr:rowOff>
+                    <xdr:rowOff>371475</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4258,15 +4331,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>373380</xdr:rowOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>47625</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4280,15 +4353,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>373380</xdr:rowOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>47625</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4302,15 +4375,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>53340</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>129540</xdr:rowOff>
+                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>373380</xdr:rowOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>47625</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4324,15 +4397,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>53340</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>129540</xdr:rowOff>
+                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>373380</xdr:rowOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>47625</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4346,15 +4419,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>373380</xdr:rowOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>47625</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4368,15 +4441,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>373380</xdr:rowOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>47625</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4390,15 +4463,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
-                    <xdr:row>9</xdr:row>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>10</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>60960</xdr:rowOff>
+                    <xdr:rowOff>219075</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4412,15 +4485,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
-                    <xdr:row>9</xdr:row>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>10</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>60960</xdr:rowOff>
+                    <xdr:rowOff>219075</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4434,15 +4507,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>53340</xdr:colOff>
-                    <xdr:row>9</xdr:row>
+                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:row>10</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>68580</xdr:rowOff>
+                    <xdr:rowOff>228600</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4456,15 +4529,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>53340</xdr:colOff>
-                    <xdr:row>9</xdr:row>
+                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:row>10</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>68580</xdr:rowOff>
+                    <xdr:rowOff>228600</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4478,15 +4551,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
-                    <xdr:row>9</xdr:row>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>10</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>60960</xdr:rowOff>
+                    <xdr:rowOff>219075</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4500,15 +4573,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
-                    <xdr:row>9</xdr:row>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>10</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>60960</xdr:rowOff>
+                    <xdr:rowOff>219075</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4522,15 +4595,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>15240</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4544,15 +4617,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>15240</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4569,11 +4642,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:R11"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="6" width="2" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
@@ -4583,11 +4656,13 @@
     <col min="12" max="12" width="15" customWidth="1"/>
     <col min="13" max="13" width="75" customWidth="1"/>
     <col min="14" max="14" width="20" customWidth="1"/>
-    <col min="15" max="17" width="30" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" customWidth="1"/>
+    <col min="16" max="16" width="21" customWidth="1"/>
+    <col min="17" max="17" width="41.85546875" customWidth="1"/>
     <col min="18" max="18" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>55</v>
       </c>
@@ -4630,7 +4705,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" ht="114.75" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
         <v>70</v>
       </c>
@@ -4657,11 +4732,15 @@
         <v>75</v>
       </c>
       <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
+      <c r="P3" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q3" s="21" t="s">
+        <v>162</v>
+      </c>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" spans="2:18" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B4" s="11"/>
       <c r="C4" s="12" t="s">
         <v>76</v>
@@ -4692,11 +4771,13 @@
         <v>83</v>
       </c>
       <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
+      <c r="P4" s="2" t="s">
+        <v>154</v>
+      </c>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="2:18" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B5" s="11"/>
       <c r="C5" s="12" t="s">
         <v>84</v>
@@ -4727,11 +4808,13 @@
         <v>90</v>
       </c>
       <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
+      <c r="P5" s="19" t="s">
+        <v>156</v>
+      </c>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="2:18" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
         <v>91</v>
@@ -4762,11 +4845,13 @@
         <v>95</v>
       </c>
       <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
+      <c r="P6" s="19" t="s">
+        <v>157</v>
+      </c>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="2:18" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B7" s="11"/>
       <c r="C7" s="12" t="s">
         <v>96</v>
@@ -4797,11 +4882,13 @@
         <v>101</v>
       </c>
       <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
+      <c r="P7" s="2" t="s">
+        <v>158</v>
+      </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="2:18" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B8" s="11"/>
       <c r="C8" s="12" t="s">
         <v>102</v>
@@ -4832,11 +4919,13 @@
         <v>107</v>
       </c>
       <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
+      <c r="P8" s="2" t="s">
+        <v>159</v>
+      </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B9" s="11"/>
       <c r="C9" s="12" t="s">
         <v>108</v>
@@ -4867,11 +4956,13 @@
         <v>112</v>
       </c>
       <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
+      <c r="P9" s="2" t="s">
+        <v>160</v>
+      </c>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B10" s="11"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -4890,7 +4981,7 @@
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
     </row>
-    <row r="11" spans="2:18" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B11" s="11"/>
       <c r="C11" s="12" t="s">
         <v>113</v>
@@ -4921,12 +5012,15 @@
         <v>118</v>
       </c>
       <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
+      <c r="P11" s="19" t="s">
+        <v>155</v>
+      </c>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="J3:J9" numberStoredAsText="1"/>
   </ignoredErrors>
@@ -4939,37 +5033,37 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="150" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="151.80000000000001" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" ht="140.25" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>124</v>
       </c>

</xml_diff>

<commit_message>
placed pregnancy yes/no into component instead of .valueBoolean
</commit_message>
<xml_diff>
--- a/Mappings/Pregnancy - STU3.xlsx
+++ b/Mappings/Pregnancy - STU3.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edelman\Nictiz-STU3-Zib2017\Mappings\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028C48AA-B353-4BBB-8723-144F58D61AC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="163">
   <si>
     <t>Subject</t>
   </si>
@@ -489,9 +483,6 @@
     <t>The fields of this HCIM fit quite well to Condition. However, the question is if Observation might be better suited. See the notes on the Data tab for more information</t>
   </si>
   <si>
-    <t>.valueBoolean</t>
-  </si>
-  <si>
     <t>.comment</t>
   </si>
   <si>
@@ -515,11 +506,14 @@
   <si>
     <t>The question is whether this HCIM maps to a Condition or an Observation. The fields map quite well on Condition and pregnancy is even mentioned as an example of a Condition. However, the intent of this HCIM is to use it as measurement of the current status, so we'll use an Observation. These observations might be grouped together in an HCIM Problem to track the overaching situation.</t>
   </si>
+  <si>
+    <t>.component / slice Pregnant (boolean)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -698,11 +692,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -864,7 +858,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -905,7 +899,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -946,7 +940,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1001,14 +995,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3073"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000010C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1016,29 +1007,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1068,14 +1036,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3074"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000020C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1083,29 +1048,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1135,14 +1077,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3075"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000030C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1150,29 +1089,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1202,14 +1118,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3076"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000040C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1217,29 +1130,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1269,14 +1159,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3077"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000050C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1284,29 +1171,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1336,14 +1200,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3078"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000060C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1351,29 +1212,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1403,14 +1241,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3079"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000070C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1418,29 +1253,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1470,14 +1282,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3080"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000080C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1485,29 +1294,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1537,14 +1323,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3081"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000090C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1552,29 +1335,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1604,14 +1364,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3082"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1619,29 +1376,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1671,14 +1405,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3083"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1686,29 +1417,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1738,14 +1446,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3084"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1753,29 +1458,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1805,14 +1487,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3085"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1820,29 +1499,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1872,14 +1528,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3086"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000E0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1887,29 +1540,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1939,14 +1569,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3087"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000F0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1954,29 +1581,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2006,14 +1610,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3088"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000100C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2021,29 +1622,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2073,14 +1651,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3089"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000110C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2088,29 +1663,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2140,14 +1692,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3090"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000120C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2155,29 +1704,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2207,14 +1733,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3091"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000130C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2222,29 +1745,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2274,14 +1774,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3092"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000140C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2289,29 +1786,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2341,14 +1815,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3093"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000150C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2356,29 +1827,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2408,14 +1856,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3094"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000160C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2423,29 +1868,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2475,14 +1897,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3095"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000170C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2490,29 +1909,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2542,14 +1938,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3096"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000180C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2557,29 +1950,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2609,14 +1979,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3097"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000190C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2624,29 +1991,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2676,14 +2020,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3098"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001A0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2691,29 +2032,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2743,14 +2061,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3099"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001B0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2758,29 +2073,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2810,14 +2102,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3100"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001C0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2825,29 +2114,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2877,14 +2143,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3101"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001D0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2892,29 +2155,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2944,14 +2184,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3102"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001E0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2959,29 +2196,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -3011,14 +2225,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3103"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001F0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3026,29 +2237,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -3078,14 +2266,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3104"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000200C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3093,29 +2278,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -3415,14 +2577,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3539,7 +2701,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -3550,7 +2712,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3562,10 +2724,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="21"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -3757,7 +2919,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3774,7 +2936,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515DB529-7A3E-4DDA-9800-41676C7906CF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4639,11 +3801,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4733,10 +3895,10 @@
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q3" s="20" t="s">
         <v>161</v>
-      </c>
-      <c r="Q3" s="21" t="s">
-        <v>162</v>
       </c>
       <c r="R3" s="4"/>
     </row>
@@ -4772,7 +3934,7 @@
       </c>
       <c r="O4" s="2"/>
       <c r="P4" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
@@ -4809,7 +3971,7 @@
       </c>
       <c r="O5" s="2"/>
       <c r="P5" s="19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
@@ -4846,7 +4008,7 @@
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
@@ -4883,7 +4045,7 @@
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
@@ -4920,7 +4082,7 @@
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
@@ -4957,7 +4119,7 @@
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
@@ -5013,7 +4175,7 @@
       </c>
       <c r="O11" s="2"/>
       <c r="P11" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
@@ -5028,7 +4190,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated mapping document with fresh insights after discussing this zib. The plan now is to use a Condition profile and attach several Observations to it
</commit_message>
<xml_diff>
--- a/Mappings/Pregnancy - STU3.xlsx
+++ b/Mappings/Pregnancy - STU3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edelman\Nictiz-STU3-Zib2017\Mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4D4C32-DEB3-4853-9B14-71387EBE99B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6582BB-F8CE-4149-A610-A36CF0220343}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="163">
   <si>
     <t>Subject</t>
   </si>
@@ -350,12 +350,6 @@
     <t>SNOMED CT: 364320009 Pregnancy observable</t>
   </si>
   <si>
-    <t>nl-core-observation (DefinitionCode on .code)</t>
-  </si>
-  <si>
-    <t>The question is whether this HCIM maps to a Condition or an Observation. The fields map quite well on Condition and pregnancy is even mentioned as an example of a Condition. However, the intent of this HCIM is to use it as measurement of the current status, so we'll use an Observation. These observations might be grouped together in an HCIM Problem to track the overaching situation.</t>
-  </si>
-  <si>
     <t>Pregnant</t>
   </si>
   <si>
@@ -380,15 +374,6 @@
     <t>SNOMED CT: 77386006 Pregnant</t>
   </si>
   <si>
-    <t>.component / slice Pregnant (boolean)</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/v2-0136</t>
-  </si>
-  <si>
-    <t>In FHUR STU3, boolean doesn’t actually exist in .component, but the official docs specify that a CodeableConcept mapping to this ValueSet  should be made as an alternative</t>
-  </si>
-  <si>
     <t>TermDate</t>
   </si>
   <si>
@@ -410,9 +395,6 @@
     <t>LOINC: 11778-8 Delivery date Estimated</t>
   </si>
   <si>
-    <t>.component / slice TermDate (DateTime)</t>
-  </si>
-  <si>
     <t>Since the DateTime data type allows for precision from whole years to microseconds, we have to make sure the actual value is a date</t>
   </si>
   <si>
@@ -431,9 +413,6 @@
     <t>SNOMED CT: 21840007 Date of last menstrual period</t>
   </si>
   <si>
-    <t>.component / slice DateLastMenstruation (DateTime)</t>
-  </si>
-  <si>
     <t>PregnancyDuration</t>
   </si>
   <si>
@@ -452,9 +431,6 @@
     <t>SNOMED CT: 57036006 Fetal gestational age</t>
   </si>
   <si>
-    <t>.component / slice PregnancyDuration (quantity)</t>
-  </si>
-  <si>
     <t>Gravidity</t>
   </si>
   <si>
@@ -473,9 +449,6 @@
     <t>LOINC: 11996-6 Pregnancies</t>
   </si>
   <si>
-    <t>.component / slice Gravidity (quantity)</t>
-  </si>
-  <si>
     <t>Parity</t>
   </si>
   <si>
@@ -491,9 +464,6 @@
     <t>LOINC: 11977-6 Parity</t>
   </si>
   <si>
-    <t>.component / slice Parity (quantity)</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -510,9 +480,6 @@
   </si>
   <si>
     <t>LOINC: 48767-8 Annotation comment</t>
-  </si>
-  <si>
-    <t>.comment</t>
   </si>
   <si>
     <t>Disclaimer</t>
@@ -538,6 +505,24 @@
 - closed slicing on Quantity.code
 - a ValueSet on Quantity.code
 We opt for the slicing approach since it is the most verbose option with the least amount of overhead</t>
+  </si>
+  <si>
+    <t>Condition.note</t>
+  </si>
+  <si>
+    <t>profiel zib-Problem (Condition)</t>
+  </si>
+  <si>
+    <t>Condition.parity (extension)</t>
+  </si>
+  <si>
+    <t>Condition.gravidity (extension)</t>
+  </si>
+  <si>
+    <t>The question is whether this HCIM maps to a Condition or an Observation. The intent of this HCIM reads as a measurement of the current status, ie an Observation, but since it might be used more widely, Condition seems to be the most appropriate. However, several of the components (pregnant yes or no, term date, date last menstruation, pregnancyduration) ARE point observations, so we'll profile them as separate obervations which refer to the Condition profile.</t>
+  </si>
+  <si>
+    <t>profile on nl-core-observation</t>
   </si>
 </sst>
 </file>
@@ -687,9 +672,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -741,6 +723,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1277,106 +1262,106 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1405,186 +1390,186 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="21"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="2"/>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1609,7 +1594,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3"/>
+      <c r="A1" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1637,119 +1622,119 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7" t="s">
+      <c r="A9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1757,12 +1742,12 @@
       <c r="D11" t="s">
         <v>85</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1776,8 +1761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1799,389 +1784,382 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="2" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="2:19" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="B3" s="12" t="s">
+    <row r="3" spans="2:19" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="B3" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="15" t="s">
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15" t="s">
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="M3" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="N3" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15" t="s">
+      <c r="O3" s="14"/>
+      <c r="P3" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="S3" s="14"/>
+    </row>
+    <row r="4" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B4" s="16"/>
+      <c r="C4" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="16" t="s">
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="S3" s="15"/>
-    </row>
-    <row r="4" spans="2:19" ht="51" x14ac:dyDescent="0.2">
-      <c r="B4" s="17"/>
-      <c r="C4" s="18" t="s">
+      <c r="I4" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="K4" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="L4" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="M4" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="N4" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="O4" s="2"/>
+      <c r="P4" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+    </row>
+    <row r="5" spans="2:19" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="B5" s="16"/>
+      <c r="C5" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="Q4" s="20" t="s">
+      <c r="J5" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="K5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="S4" s="3"/>
-    </row>
-    <row r="5" spans="2:19" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="B5" s="17"/>
-      <c r="C5" s="18" t="s">
+      <c r="M5" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="3" t="s">
+      <c r="N5" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="O5" s="2"/>
+      <c r="P5" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="J5" s="3" t="s">
+    </row>
+    <row r="6" spans="2:19" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="B6" s="16"/>
+      <c r="C6" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="L5" s="3" t="s">
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="I6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="M6" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="O5" s="3"/>
-      <c r="P5" s="21" t="s">
+      <c r="N6" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3" t="s">
+      <c r="O6" s="2"/>
+      <c r="P6" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" ht="102" x14ac:dyDescent="0.2">
+      <c r="B7" s="16"/>
+      <c r="C7" s="17" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="6" spans="2:19" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="B6" s="17"/>
-      <c r="C6" s="18" t="s">
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="3" t="s">
+      <c r="I7" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="L6" s="3" t="s">
+      <c r="J7" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M7" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N7" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="O6" s="3"/>
-      <c r="P6" s="21" t="s">
+      <c r="O7" s="2"/>
+      <c r="P7" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="S7" s="2"/>
+    </row>
+    <row r="8" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B8" s="16"/>
+      <c r="C8" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="2:19" ht="102" x14ac:dyDescent="0.2">
-      <c r="B7" s="17"/>
-      <c r="C7" s="18" t="s">
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="3" t="s">
+      <c r="I8" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J8" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="L7" s="3" t="s">
+      <c r="M8" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="N8" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="O8" s="2"/>
+      <c r="P8" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+    </row>
+    <row r="9" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B9" s="16"/>
+      <c r="C9" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3" t="s">
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="S7" s="3"/>
-    </row>
-    <row r="8" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B8" s="17"/>
-      <c r="C8" s="18" t="s">
+      <c r="I9" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="3" t="s">
+      <c r="M9" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="N9" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="L8" s="3" t="s">
+      <c r="O9" s="2"/>
+      <c r="P9" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B10" s="16"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+    </row>
+    <row r="11" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B11" s="16"/>
+      <c r="C11" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="I11" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3" t="s">
+      <c r="J11" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-    </row>
-    <row r="9" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B9" s="17"/>
-      <c r="C9" s="18" t="s">
+      <c r="M11" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="3" t="s">
+      <c r="N11" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-    </row>
-    <row r="11" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B11" s="17"/>
-      <c r="C11" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="L11" s="3" t="s">
+      <c r="O11" s="2"/>
+      <c r="P11" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="M11" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="O11" s="3"/>
-      <c r="P11" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="Q4" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2199,33 +2177,33 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
-        <v>161</v>
+      <c r="B2" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
-        <v>162</v>
+      <c r="B3" s="2" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
-        <v>163</v>
+      <c r="B4" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
-        <v>164</v>
+      <c r="B5" s="2" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
-        <v>165</v>
+      <c r="B6" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
-        <v>166</v>
+      <c r="B7" s="2" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>